<commit_message>
login test for Swag bag added
</commit_message>
<xml_diff>
--- a/softinnovas/testingData.xlsx
+++ b/softinnovas/testingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayru\eclipse-workspace\selenium\java-selenium-learning\softinnovas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC0E13D-828A-4E80-AE22-DC78BA45A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3479BC39-C36C-438D-BD53-ADBF5567A274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{737D6610-2D41-4936-B807-6DF3F2553FE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{737D6610-2D41-4936-B807-6DF3F2553FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Leads" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>FirstName</t>
   </si>
@@ -177,10 +177,19 @@
     <t>Type</t>
   </si>
   <si>
-    <t>KKKKK</t>
-  </si>
-  <si>
-    <t>AAAA</t>
+    <t>CCL Industries Inc</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>Aa</t>
+  </si>
+  <si>
+    <t>AAR Corp</t>
   </si>
 </sst>
 </file>
@@ -545,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B823BEBB-D72F-4650-8125-FAEB29AA69AE}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G2">
         <v>5555555555</v>
@@ -644,7 +653,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>1111111111</v>
@@ -735,13 +744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7151B789-BB7A-4DD0-8DAE-DF546185E822}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -750,7 +757,7 @@
         <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -761,18 +768,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2">
-        <v>5128888558</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3">
-        <v>8745963252</v>
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>